<commit_message>
refreshing - create standalone python code 1
</commit_message>
<xml_diff>
--- a/revenue-streamlit/tenancy_list_scenario_02b.xlsx
+++ b/revenue-streamlit/tenancy_list_scenario_02b.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mawan/Development/office/revenue-streamlit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8db03e8e420626a2/Office/AMG/Development/office/revenue-streamlit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736FF6E1-3601-A345-8876-257CE5B3F247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{736FF6E1-3601-A345-8876-257CE5B3F247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B6597E4-E2FF-4D48-B35A-797FF7098BDD}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="1040" windowWidth="30820" windowHeight="22340" tabRatio="765" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="880" windowWidth="30820" windowHeight="21500" tabRatio="765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="2" r:id="rId1"/>
@@ -1537,7 +1537,177 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="71">
+  <dxfs count="56">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -1546,228 +1716,6 @@
         <right/>
         <top style="thin">
           <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;_);_(@_)"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
         </top>
         <bottom/>
       </border>
@@ -1789,6 +1737,21 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1831,6 +1794,21 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1870,6 +1848,21 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
       <fill>
         <patternFill patternType="none">
@@ -1891,6 +1884,21 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1930,6 +1938,21 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1973,6 +1996,22 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;_);_(@_)"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2009,6 +2048,21 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2051,6 +2105,35 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2069,6 +2152,21 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2095,6 +2193,21 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -2115,6 +2228,21 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2157,6 +2285,35 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor rgb="FF000000"/>
@@ -2173,6 +2330,19 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2250,290 +2420,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2553,13 +2439,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>246807</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>132619</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>288616</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>77683</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -2631,13 +2517,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>234894</xdr:colOff>
-      <xdr:row>169</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>86989</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>276703</xdr:colOff>
-      <xdr:row>182</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>32053</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -2709,13 +2595,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>222981</xdr:colOff>
-      <xdr:row>182</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>131271</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>264790</xdr:colOff>
-      <xdr:row>203</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>157345</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
@@ -2820,42 +2706,31 @@
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
   <slicer name="Product_Type" xr10:uid="{3E27C4DA-B740-D643-BDF7-575D40894E0A}" cache="Slicer_Product_Type" caption="Product_Type" rowHeight="230716"/>
   <slicer name="Group" xr10:uid="{40B0A4B9-B561-5347-8FF6-F50F053C1A4C}" cache="Slicer_Group" caption="Group" rowHeight="230716"/>
-  <slicer name="End" xr10:uid="{B17BD57E-B2EA-1042-9987-3412CB8A8925}" cache="Slicer_End" caption="End" startItem="11" rowHeight="230716"/>
+  <slicer name="End" xr10:uid="{B17BD57E-B2EA-1042-9987-3412CB8A8925}" cache="Slicer_End" caption="End" rowHeight="230716"/>
 </slicers>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A0023E2-6AF7-7B4C-AA3C-5526EA8C01E9}" name="Table1" displayName="Table1" ref="A1:N161" totalsRowCount="1" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" totalsRowBorderDxfId="28">
-  <autoFilter ref="A1:N160" xr:uid="{1A0023E2-6AF7-7B4C-AA3C-5526EA8C01E9}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="19"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Office"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A0023E2-6AF7-7B4C-AA3C-5526EA8C01E9}" name="Table1" displayName="Table1" ref="A1:N161" totalsRowCount="1" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+  <autoFilter ref="A1:N160" xr:uid="{1A0023E2-6AF7-7B4C-AA3C-5526EA8C01E9}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N132">
     <sortCondition descending="1" ref="C3:C132"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{82702CBB-B7D8-5C45-8EE8-39144A9E6839}" name="No" totalsRowLabel="Total" dataDxfId="27" totalsRowDxfId="13"/>
-    <tableColumn id="13" xr3:uid="{81693DE1-7410-4E03-8801-E72BA5AA4D0C}" name="Location" dataDxfId="26" totalsRowDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{49AC1DFB-968F-8C4C-B46A-BA65A08A82F8}" name="Floor" dataDxfId="25" totalsRowDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{7407A2D4-11A2-B14C-9C1E-EB812BA07976}" name="Zone" dataDxfId="24" totalsRowDxfId="10"/>
-    <tableColumn id="11" xr3:uid="{EDDF5F0D-2514-4DA3-8E09-CC07C1F5EC73}" name="Product_Type" dataDxfId="23" totalsRowDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{584F12DA-F9A2-F044-BEE3-95C850B08187}" name="Group" dataDxfId="22" totalsRowDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{9F70DA22-AD03-2E40-982C-172221ED7B17}" name="Tenant" dataDxfId="21" totalsRowDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{38FEB9FC-3468-1746-8CEA-0778DBB66ECF}" name="Area" dataDxfId="20" totalsRowDxfId="6" dataCellStyle="Comma"/>
-    <tableColumn id="9" xr3:uid="{D64C9D1A-FA8B-4C4D-B607-52E1E05305B0}" name="Chg_Type" dataDxfId="19" totalsRowDxfId="5" dataCellStyle="Comma"/>
-    <tableColumn id="7" xr3:uid="{CFF86D67-BC6E-F940-B6C5-060702DC8E14}" name="Start" dataDxfId="18" totalsRowDxfId="4" dataCellStyle="Comma"/>
-    <tableColumn id="8" xr3:uid="{A0B757F2-99D8-6B48-9212-0A3F40DF200F}" name="End" dataDxfId="17" totalsRowDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{29206E0A-C3D4-7148-A9B7-062237C9AD9C}" name="Rental_Rate" dataDxfId="16" totalsRowDxfId="2" dataCellStyle="Comma [0]"/>
-    <tableColumn id="12" xr3:uid="{6631B20D-5386-3149-B067-110BB05C3B0A}" name="SC_Rate" dataDxfId="15" totalsRowDxfId="1" dataCellStyle="Comma [0]"/>
-    <tableColumn id="5" xr3:uid="{61759F5E-0021-784D-BB1B-F0F0AD385D08}" name="Notes_1" dataDxfId="14" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{82702CBB-B7D8-5C45-8EE8-39144A9E6839}" name="No" totalsRowLabel="Total" dataDxfId="50" totalsRowDxfId="49"/>
+    <tableColumn id="13" xr3:uid="{81693DE1-7410-4E03-8801-E72BA5AA4D0C}" name="Location" dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{49AC1DFB-968F-8C4C-B46A-BA65A08A82F8}" name="Floor" dataDxfId="46" totalsRowDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{7407A2D4-11A2-B14C-9C1E-EB812BA07976}" name="Zone" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="11" xr3:uid="{EDDF5F0D-2514-4DA3-8E09-CC07C1F5EC73}" name="Product_Type" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="14" xr3:uid="{584F12DA-F9A2-F044-BEE3-95C850B08187}" name="Group" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{9F70DA22-AD03-2E40-982C-172221ED7B17}" name="Tenant" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{38FEB9FC-3468-1746-8CEA-0778DBB66ECF}" name="Area" dataDxfId="36" totalsRowDxfId="35" dataCellStyle="Comma"/>
+    <tableColumn id="9" xr3:uid="{D64C9D1A-FA8B-4C4D-B607-52E1E05305B0}" name="Chg_Type" dataDxfId="34" totalsRowDxfId="33" dataCellStyle="Comma"/>
+    <tableColumn id="7" xr3:uid="{CFF86D67-BC6E-F940-B6C5-060702DC8E14}" name="Start" dataDxfId="32" totalsRowDxfId="31" dataCellStyle="Comma"/>
+    <tableColumn id="8" xr3:uid="{A0B757F2-99D8-6B48-9212-0A3F40DF200F}" name="End" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="10" xr3:uid="{29206E0A-C3D4-7148-A9B7-062237C9AD9C}" name="Rental_Rate" dataDxfId="28" totalsRowDxfId="27" dataCellStyle="Comma [0]"/>
+    <tableColumn id="12" xr3:uid="{6631B20D-5386-3149-B067-110BB05C3B0A}" name="SC_Rate" dataDxfId="26" totalsRowDxfId="25" dataCellStyle="Comma [0]"/>
+    <tableColumn id="5" xr3:uid="{61759F5E-0021-784D-BB1B-F0F0AD385D08}" name="Notes_1" dataDxfId="24" totalsRowDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3160,8 +3035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:J7"/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3235,7 +3110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N161"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="113" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="113" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="K188" sqref="K188"/>
     </sheetView>
   </sheetViews>
@@ -3298,7 +3173,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="29">
         <v>1</v>
       </c>
@@ -3340,7 +3215,7 @@
       </c>
       <c r="N2" s="20"/>
     </row>
-    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="29">
         <v>2</v>
       </c>
@@ -3383,7 +3258,7 @@
       </c>
       <c r="N3" s="20"/>
     </row>
-    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="29">
         <v>3</v>
       </c>
@@ -3426,7 +3301,7 @@
       </c>
       <c r="N4" s="20"/>
     </row>
-    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="29">
         <v>4</v>
       </c>
@@ -3469,7 +3344,7 @@
       </c>
       <c r="N5" s="20"/>
     </row>
-    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="29">
         <v>5</v>
       </c>
@@ -3510,7 +3385,7 @@
       </c>
       <c r="N6" s="20"/>
     </row>
-    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="29">
         <v>6</v>
       </c>
@@ -3553,7 +3428,7 @@
       </c>
       <c r="N7" s="20"/>
     </row>
-    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="29">
         <v>7</v>
       </c>
@@ -3596,7 +3471,7 @@
       </c>
       <c r="N8" s="20"/>
     </row>
-    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="29">
         <v>8</v>
       </c>
@@ -3639,7 +3514,7 @@
       </c>
       <c r="N9" s="20"/>
     </row>
-    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="29">
         <v>9</v>
       </c>
@@ -3682,7 +3557,7 @@
       </c>
       <c r="N10" s="20"/>
     </row>
-    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="29">
         <v>10</v>
       </c>
@@ -3725,7 +3600,7 @@
       </c>
       <c r="N11" s="20"/>
     </row>
-    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="29">
         <v>11</v>
       </c>
@@ -3768,7 +3643,7 @@
       </c>
       <c r="N12" s="20"/>
     </row>
-    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="29">
         <v>12</v>
       </c>
@@ -3811,7 +3686,7 @@
       </c>
       <c r="N13" s="20"/>
     </row>
-    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="29">
         <v>14</v>
       </c>
@@ -3853,7 +3728,7 @@
       </c>
       <c r="N14" s="20"/>
     </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="29">
         <v>15</v>
       </c>
@@ -3895,7 +3770,7 @@
       </c>
       <c r="N15" s="20"/>
     </row>
-    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="29">
         <v>13</v>
       </c>
@@ -3938,7 +3813,7 @@
       </c>
       <c r="N16" s="20"/>
     </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="29">
         <v>18</v>
       </c>
@@ -3974,7 +3849,7 @@
       <c r="M17" s="14"/>
       <c r="N17" s="20"/>
     </row>
-    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="29">
         <v>16</v>
       </c>
@@ -4018,7 +3893,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="29">
         <v>17</v>
       </c>
@@ -4060,7 +3935,7 @@
       </c>
       <c r="N19" s="20"/>
     </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="29">
         <v>19</v>
       </c>
@@ -4096,7 +3971,7 @@
       <c r="M20" s="40"/>
       <c r="N20" s="20"/>
     </row>
-    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="29">
         <v>20</v>
       </c>
@@ -4132,7 +4007,7 @@
       <c r="M21" s="40"/>
       <c r="N21" s="20"/>
     </row>
-    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="29">
         <v>22</v>
       </c>
@@ -4174,7 +4049,7 @@
       </c>
       <c r="N22" s="20"/>
     </row>
-    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="29">
         <v>21</v>
       </c>
@@ -4216,7 +4091,7 @@
       </c>
       <c r="N23" s="20"/>
     </row>
-    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="29">
         <v>23</v>
       </c>
@@ -4252,7 +4127,7 @@
       <c r="M24" s="6"/>
       <c r="N24" s="20"/>
     </row>
-    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="29">
         <v>25</v>
       </c>
@@ -4294,7 +4169,7 @@
       </c>
       <c r="N25" s="20"/>
     </row>
-    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="29">
         <v>24</v>
       </c>
@@ -4334,7 +4209,7 @@
       </c>
       <c r="N26" s="20"/>
     </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="29">
         <v>26</v>
       </c>
@@ -4374,7 +4249,7 @@
       </c>
       <c r="N27" s="20"/>
     </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="29">
         <v>27</v>
       </c>
@@ -4416,7 +4291,7 @@
       </c>
       <c r="N28" s="20"/>
     </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="29">
         <v>28</v>
       </c>
@@ -4459,7 +4334,7 @@
       </c>
       <c r="N29" s="20"/>
     </row>
-    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="29">
         <v>29</v>
       </c>
@@ -4501,7 +4376,7 @@
       </c>
       <c r="N30" s="20"/>
     </row>
-    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="29">
         <v>30</v>
       </c>
@@ -4537,7 +4412,7 @@
       <c r="M31" s="6"/>
       <c r="N31" s="20"/>
     </row>
-    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="29">
         <v>31</v>
       </c>
@@ -4579,7 +4454,7 @@
       </c>
       <c r="N32" s="20"/>
     </row>
-    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="29">
         <v>32</v>
       </c>
@@ -4621,7 +4496,7 @@
       </c>
       <c r="N33" s="20"/>
     </row>
-    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="29"/>
       <c r="B34" s="29" t="s">
         <v>177</v>
@@ -4661,7 +4536,7 @@
       </c>
       <c r="N34" s="20"/>
     </row>
-    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="29"/>
       <c r="B35" s="29" t="s">
         <v>177</v>
@@ -4701,7 +4576,7 @@
       </c>
       <c r="N35" s="20"/>
     </row>
-    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="29">
         <v>33</v>
       </c>
@@ -4743,7 +4618,7 @@
       </c>
       <c r="N36" s="20"/>
     </row>
-    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="29">
         <v>34</v>
       </c>
@@ -4779,7 +4654,7 @@
       <c r="M37" s="6"/>
       <c r="N37" s="20"/>
     </row>
-    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="29">
         <v>39</v>
       </c>
@@ -4821,7 +4696,7 @@
       </c>
       <c r="N38" s="20"/>
     </row>
-    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="29">
         <v>37</v>
       </c>
@@ -4863,7 +4738,7 @@
       </c>
       <c r="N39" s="20"/>
     </row>
-    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="29">
         <v>36</v>
       </c>
@@ -4905,7 +4780,7 @@
       </c>
       <c r="N40" s="20"/>
     </row>
-    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="29">
         <v>38</v>
       </c>
@@ -4941,7 +4816,7 @@
       <c r="M41" s="6"/>
       <c r="N41" s="20"/>
     </row>
-    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="29">
         <v>35</v>
       </c>
@@ -4983,7 +4858,7 @@
       </c>
       <c r="N42" s="20"/>
     </row>
-    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="29">
         <v>46</v>
       </c>
@@ -5026,7 +4901,7 @@
       </c>
       <c r="N43" s="20"/>
     </row>
-    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="29">
         <v>42</v>
       </c>
@@ -5068,7 +4943,7 @@
       </c>
       <c r="N44" s="20"/>
     </row>
-    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="29">
         <v>43</v>
       </c>
@@ -5104,7 +4979,7 @@
       <c r="M45" s="40"/>
       <c r="N45" s="20"/>
     </row>
-    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="29">
         <v>44</v>
       </c>
@@ -5144,7 +5019,7 @@
       </c>
       <c r="N46" s="20"/>
     </row>
-    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="29">
         <v>41</v>
       </c>
@@ -5186,7 +5061,7 @@
       </c>
       <c r="N47" s="20"/>
     </row>
-    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="29">
         <v>45</v>
       </c>
@@ -5222,7 +5097,7 @@
       <c r="M48" s="6"/>
       <c r="N48" s="20"/>
     </row>
-    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="29">
         <v>47</v>
       </c>
@@ -5264,7 +5139,7 @@
       </c>
       <c r="N49" s="20"/>
     </row>
-    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="29">
         <v>40</v>
       </c>
@@ -5306,7 +5181,7 @@
       </c>
       <c r="N50" s="20"/>
     </row>
-    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="29">
         <v>48</v>
       </c>
@@ -5348,7 +5223,7 @@
       </c>
       <c r="N51" s="20"/>
     </row>
-    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="29">
         <v>49</v>
       </c>
@@ -5390,7 +5265,7 @@
       </c>
       <c r="N52" s="20"/>
     </row>
-    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="29">
         <v>50</v>
       </c>
@@ -5432,7 +5307,7 @@
       </c>
       <c r="N53" s="20"/>
     </row>
-    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="29">
         <v>51</v>
       </c>
@@ -5475,7 +5350,7 @@
       </c>
       <c r="N54" s="20"/>
     </row>
-    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="29">
         <v>53</v>
       </c>
@@ -5517,7 +5392,7 @@
       </c>
       <c r="N55" s="20"/>
     </row>
-    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="29">
         <v>52</v>
       </c>
@@ -5559,7 +5434,7 @@
       </c>
       <c r="N56" s="20"/>
     </row>
-    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="29">
         <v>55</v>
       </c>
@@ -5595,7 +5470,7 @@
       <c r="M57" s="6"/>
       <c r="N57" s="20"/>
     </row>
-    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="29">
         <v>54</v>
       </c>
@@ -5637,7 +5512,7 @@
       </c>
       <c r="N58" s="20"/>
     </row>
-    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="29">
         <v>56</v>
       </c>
@@ -5673,7 +5548,7 @@
       <c r="M59" s="6"/>
       <c r="N59" s="20"/>
     </row>
-    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="29">
         <v>57</v>
       </c>
@@ -5953,7 +5828,7 @@
       </c>
       <c r="N66" s="20"/>
     </row>
-    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="29">
         <v>63</v>
       </c>
@@ -5995,7 +5870,7 @@
       </c>
       <c r="N67" s="20"/>
     </row>
-    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="29">
         <v>65</v>
       </c>
@@ -6037,7 +5912,7 @@
       </c>
       <c r="N68" s="20"/>
     </row>
-    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="29">
         <v>64</v>
       </c>
@@ -6079,7 +5954,7 @@
       </c>
       <c r="N69" s="20"/>
     </row>
-    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="29">
         <v>66</v>
       </c>
@@ -6121,7 +5996,7 @@
       </c>
       <c r="N70" s="20"/>
     </row>
-    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="29">
         <v>67</v>
       </c>
@@ -6157,7 +6032,7 @@
       <c r="M71" s="6"/>
       <c r="N71" s="20"/>
     </row>
-    <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="29">
         <v>68</v>
       </c>
@@ -6199,7 +6074,7 @@
       </c>
       <c r="N72" s="20"/>
     </row>
-    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="29">
         <v>69</v>
       </c>
@@ -6241,7 +6116,7 @@
       </c>
       <c r="N73" s="20"/>
     </row>
-    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="29">
         <v>70</v>
       </c>
@@ -6283,7 +6158,7 @@
       </c>
       <c r="N74" s="20"/>
     </row>
-    <row r="75" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="29">
         <v>71</v>
       </c>
@@ -6319,7 +6194,7 @@
       <c r="M75" s="6"/>
       <c r="N75" s="20"/>
     </row>
-    <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="29">
         <v>72</v>
       </c>
@@ -6361,7 +6236,7 @@
       </c>
       <c r="N76" s="20"/>
     </row>
-    <row r="77" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="29">
         <v>73</v>
       </c>
@@ -6397,7 +6272,7 @@
       <c r="M77" s="6"/>
       <c r="N77" s="20"/>
     </row>
-    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="29">
         <v>77</v>
       </c>
@@ -6439,7 +6314,7 @@
       </c>
       <c r="N78" s="20"/>
     </row>
-    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="29">
         <v>74</v>
       </c>
@@ -6481,7 +6356,7 @@
       </c>
       <c r="N79" s="20"/>
     </row>
-    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="29">
         <v>81</v>
       </c>
@@ -6517,7 +6392,7 @@
       <c r="M80" s="6"/>
       <c r="N80" s="20"/>
     </row>
-    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="29">
         <v>79</v>
       </c>
@@ -6559,7 +6434,7 @@
       </c>
       <c r="N81" s="20"/>
     </row>
-    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="29">
         <v>75</v>
       </c>
@@ -6601,7 +6476,7 @@
       </c>
       <c r="N82" s="20"/>
     </row>
-    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="29">
         <v>82</v>
       </c>
@@ -6637,7 +6512,7 @@
       <c r="M83" s="6"/>
       <c r="N83" s="20"/>
     </row>
-    <row r="84" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="29">
         <v>85</v>
       </c>
@@ -6677,7 +6552,7 @@
       </c>
       <c r="N84" s="20"/>
     </row>
-    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="29">
         <v>86</v>
       </c>
@@ -6717,7 +6592,7 @@
       </c>
       <c r="N85" s="20"/>
     </row>
-    <row r="86" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="29">
         <v>76</v>
       </c>
@@ -6759,7 +6634,7 @@
       </c>
       <c r="N86" s="20"/>
     </row>
-    <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="29">
         <v>83</v>
       </c>
@@ -6795,7 +6670,7 @@
       <c r="M87" s="6"/>
       <c r="N87" s="20"/>
     </row>
-    <row r="88" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="29">
         <v>80</v>
       </c>
@@ -6840,7 +6715,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="29">
         <v>78</v>
       </c>
@@ -6882,7 +6757,7 @@
       </c>
       <c r="N89" s="20"/>
     </row>
-    <row r="90" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="29">
         <v>84</v>
       </c>
@@ -6918,7 +6793,7 @@
       <c r="M90" s="6"/>
       <c r="N90" s="20"/>
     </row>
-    <row r="91" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="29">
         <v>91</v>
       </c>
@@ -6958,7 +6833,7 @@
       </c>
       <c r="N91" s="20"/>
     </row>
-    <row r="92" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="29"/>
       <c r="B92" s="29" t="s">
         <v>177</v>
@@ -6992,7 +6867,7 @@
       <c r="M92" s="6"/>
       <c r="N92" s="20"/>
     </row>
-    <row r="93" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="29">
         <v>94</v>
       </c>
@@ -7034,7 +6909,7 @@
       </c>
       <c r="N93" s="20"/>
     </row>
-    <row r="94" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="29">
         <v>90</v>
       </c>
@@ -7076,7 +6951,7 @@
       </c>
       <c r="N94" s="20"/>
     </row>
-    <row r="95" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" s="29">
         <v>92</v>
       </c>
@@ -7112,7 +6987,7 @@
       <c r="M95" s="6"/>
       <c r="N95" s="20"/>
     </row>
-    <row r="96" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" s="29">
         <v>88</v>
       </c>
@@ -7154,7 +7029,7 @@
       </c>
       <c r="N96" s="20"/>
     </row>
-    <row r="97" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" s="29">
         <v>87</v>
       </c>
@@ -7196,7 +7071,7 @@
       </c>
       <c r="N97" s="20"/>
     </row>
-    <row r="98" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" s="29">
         <v>95</v>
       </c>
@@ -7238,7 +7113,7 @@
       </c>
       <c r="N98" s="20"/>
     </row>
-    <row r="99" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" s="29">
         <v>96</v>
       </c>
@@ -7280,7 +7155,7 @@
       </c>
       <c r="N99" s="20"/>
     </row>
-    <row r="100" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" s="29">
         <v>97</v>
       </c>
@@ -7322,7 +7197,7 @@
       </c>
       <c r="N100" s="20"/>
     </row>
-    <row r="101" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" s="29">
         <v>98</v>
       </c>
@@ -7362,7 +7237,7 @@
       </c>
       <c r="N101" s="20"/>
     </row>
-    <row r="102" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" s="29">
         <v>100</v>
       </c>
@@ -7404,7 +7279,7 @@
       </c>
       <c r="N102" s="20"/>
     </row>
-    <row r="103" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="29">
         <v>99</v>
       </c>
@@ -7444,7 +7319,7 @@
       </c>
       <c r="N103" s="20"/>
     </row>
-    <row r="104" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" s="29">
         <v>101</v>
       </c>
@@ -7486,7 +7361,7 @@
       </c>
       <c r="N104" s="20"/>
     </row>
-    <row r="105" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" s="29">
         <v>102</v>
       </c>
@@ -7526,7 +7401,7 @@
       </c>
       <c r="N105" s="20"/>
     </row>
-    <row r="106" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" s="29">
         <v>103</v>
       </c>
@@ -7568,7 +7443,7 @@
       </c>
       <c r="N106" s="20"/>
     </row>
-    <row r="107" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" s="29">
         <v>104</v>
       </c>
@@ -7608,7 +7483,7 @@
       </c>
       <c r="N107" s="20"/>
     </row>
-    <row r="108" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" s="29">
         <v>105</v>
       </c>
@@ -7650,7 +7525,7 @@
       </c>
       <c r="N108" s="20"/>
     </row>
-    <row r="109" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" s="29">
         <v>106</v>
       </c>
@@ -7686,7 +7561,7 @@
       <c r="M109" s="14"/>
       <c r="N109" s="20"/>
     </row>
-    <row r="110" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" s="29">
         <v>107</v>
       </c>
@@ -7722,7 +7597,7 @@
       <c r="M110" s="14"/>
       <c r="N110" s="20"/>
     </row>
-    <row r="111" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" s="29">
         <v>108</v>
       </c>
@@ -7764,7 +7639,7 @@
       </c>
       <c r="N111" s="20"/>
     </row>
-    <row r="112" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" s="29">
         <v>109</v>
       </c>
@@ -7806,7 +7681,7 @@
       </c>
       <c r="N112" s="20"/>
     </row>
-    <row r="113" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" s="29">
         <v>110</v>
       </c>
@@ -7848,7 +7723,7 @@
       </c>
       <c r="N113" s="20"/>
     </row>
-    <row r="114" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="29">
         <v>111</v>
       </c>
@@ -7890,7 +7765,7 @@
       </c>
       <c r="N114" s="20"/>
     </row>
-    <row r="115" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="29">
         <v>112</v>
       </c>
@@ -7932,7 +7807,7 @@
       </c>
       <c r="N115" s="20"/>
     </row>
-    <row r="116" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" s="29">
         <v>113</v>
       </c>
@@ -7974,7 +7849,7 @@
       </c>
       <c r="N116" s="20"/>
     </row>
-    <row r="117" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" s="29">
         <v>114</v>
       </c>
@@ -8016,7 +7891,7 @@
       </c>
       <c r="N117" s="20"/>
     </row>
-    <row r="118" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" s="29">
         <v>115</v>
       </c>
@@ -8058,7 +7933,7 @@
       </c>
       <c r="N118" s="20"/>
     </row>
-    <row r="119" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" s="29">
         <v>116</v>
       </c>
@@ -8100,7 +7975,7 @@
       </c>
       <c r="N119" s="20"/>
     </row>
-    <row r="120" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" s="29">
         <v>117</v>
       </c>
@@ -8136,7 +8011,7 @@
       <c r="M120" s="14"/>
       <c r="N120" s="20"/>
     </row>
-    <row r="121" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" s="29">
         <v>118</v>
       </c>
@@ -8172,7 +8047,7 @@
       <c r="M121" s="14"/>
       <c r="N121" s="20"/>
     </row>
-    <row r="122" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" s="29">
         <v>119</v>
       </c>
@@ -8208,7 +8083,7 @@
       <c r="M122" s="15"/>
       <c r="N122" s="20"/>
     </row>
-    <row r="123" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" s="29">
         <v>120</v>
       </c>
@@ -8250,7 +8125,7 @@
       </c>
       <c r="N123" s="20"/>
     </row>
-    <row r="124" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" s="29">
         <v>121</v>
       </c>
@@ -8292,7 +8167,7 @@
       </c>
       <c r="N124" s="20"/>
     </row>
-    <row r="125" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" s="29">
         <v>122</v>
       </c>
@@ -8334,7 +8209,7 @@
       </c>
       <c r="N125" s="20"/>
     </row>
-    <row r="126" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" s="29">
         <v>123</v>
       </c>
@@ -8376,7 +8251,7 @@
       </c>
       <c r="N126" s="20"/>
     </row>
-    <row r="127" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" s="29">
         <v>124</v>
       </c>
@@ -8418,7 +8293,7 @@
       </c>
       <c r="N127" s="20"/>
     </row>
-    <row r="128" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" s="29">
         <v>125</v>
       </c>
@@ -8452,7 +8327,7 @@
       <c r="M128" s="14"/>
       <c r="N128" s="20"/>
     </row>
-    <row r="129" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" s="29">
         <v>126</v>
       </c>
@@ -8492,7 +8367,7 @@
       </c>
       <c r="N129" s="20"/>
     </row>
-    <row r="130" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" s="29">
         <v>127</v>
       </c>
@@ -8532,7 +8407,7 @@
       </c>
       <c r="N130" s="20"/>
     </row>
-    <row r="131" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" s="29">
         <v>128</v>
       </c>
@@ -8572,7 +8447,7 @@
       </c>
       <c r="N131" s="20"/>
     </row>
-    <row r="132" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" s="29">
         <v>129</v>
       </c>
@@ -8614,7 +8489,7 @@
       </c>
       <c r="N132" s="20"/>
     </row>
-    <row r="133" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133" s="29">
         <v>130</v>
       </c>
@@ -8656,7 +8531,7 @@
       </c>
       <c r="N133" s="20"/>
     </row>
-    <row r="134" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" s="29">
         <v>131</v>
       </c>
@@ -8696,7 +8571,7 @@
       <c r="M134" s="15"/>
       <c r="N134" s="20"/>
     </row>
-    <row r="135" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135" s="29">
         <v>132</v>
       </c>
@@ -8736,7 +8611,7 @@
       <c r="M135" s="15"/>
       <c r="N135" s="20"/>
     </row>
-    <row r="136" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136" s="29">
         <v>133</v>
       </c>
@@ -8778,7 +8653,7 @@
       </c>
       <c r="N136" s="20"/>
     </row>
-    <row r="137" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" s="29">
         <v>134</v>
       </c>
@@ -8820,7 +8695,7 @@
       </c>
       <c r="N137" s="20"/>
     </row>
-    <row r="138" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138" s="29">
         <v>135</v>
       </c>
@@ -8860,7 +8735,7 @@
       <c r="M138" s="15"/>
       <c r="N138" s="20"/>
     </row>
-    <row r="139" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139" s="29">
         <v>136</v>
       </c>
@@ -8900,7 +8775,7 @@
       <c r="M139" s="15"/>
       <c r="N139" s="20"/>
     </row>
-    <row r="140" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140" s="29">
         <v>137</v>
       </c>
@@ -8942,7 +8817,7 @@
       </c>
       <c r="N140" s="20"/>
     </row>
-    <row r="141" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141" s="29">
         <v>138</v>
       </c>
@@ -8984,7 +8859,7 @@
       </c>
       <c r="N141" s="20"/>
     </row>
-    <row r="142" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142" s="29">
         <v>139</v>
       </c>
@@ -9024,7 +8899,7 @@
       <c r="M142" s="15"/>
       <c r="N142" s="20"/>
     </row>
-    <row r="143" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143" s="29">
         <v>140</v>
       </c>
@@ -9064,7 +8939,7 @@
       <c r="M143" s="15"/>
       <c r="N143" s="20"/>
     </row>
-    <row r="144" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144" s="29">
         <v>141</v>
       </c>
@@ -9106,7 +8981,7 @@
       </c>
       <c r="N144" s="20"/>
     </row>
-    <row r="145" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145" s="29">
         <v>142</v>
       </c>
@@ -9148,7 +9023,7 @@
       </c>
       <c r="N145" s="20"/>
     </row>
-    <row r="146" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146" s="29">
         <v>143</v>
       </c>
@@ -9182,7 +9057,7 @@
       </c>
       <c r="N146" s="20"/>
     </row>
-    <row r="147" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A147" s="29">
         <v>144</v>
       </c>
@@ -9224,7 +9099,7 @@
       </c>
       <c r="N147" s="20"/>
     </row>
-    <row r="148" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A148" s="29">
         <v>145</v>
       </c>
@@ -9264,7 +9139,7 @@
       <c r="M148" s="15"/>
       <c r="N148" s="20"/>
     </row>
-    <row r="149" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A149" s="29">
         <v>146</v>
       </c>
@@ -9304,7 +9179,7 @@
       <c r="M149" s="14"/>
       <c r="N149" s="20"/>
     </row>
-    <row r="150" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A150" s="29">
         <v>147</v>
       </c>
@@ -9344,7 +9219,7 @@
       <c r="M150" s="14"/>
       <c r="N150" s="20"/>
     </row>
-    <row r="151" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A151" s="29">
         <v>148</v>
       </c>
@@ -9380,7 +9255,7 @@
       <c r="M151" s="15"/>
       <c r="N151" s="20"/>
     </row>
-    <row r="152" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A152" s="29">
         <v>149</v>
       </c>
@@ -9416,7 +9291,7 @@
       <c r="M152" s="15"/>
       <c r="N152" s="20"/>
     </row>
-    <row r="153" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153" s="29">
         <v>150</v>
       </c>
@@ -9452,7 +9327,7 @@
       <c r="M153" s="15"/>
       <c r="N153" s="20"/>
     </row>
-    <row r="154" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A154" s="29">
         <v>151</v>
       </c>
@@ -9488,7 +9363,7 @@
       <c r="M154" s="15"/>
       <c r="N154" s="20"/>
     </row>
-    <row r="155" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A155" s="29">
         <v>152</v>
       </c>
@@ -9524,7 +9399,7 @@
       <c r="M155" s="15"/>
       <c r="N155" s="20"/>
     </row>
-    <row r="156" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156" s="29">
         <v>153</v>
       </c>
@@ -9560,7 +9435,7 @@
       <c r="M156" s="15"/>
       <c r="N156" s="20"/>
     </row>
-    <row r="157" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157" s="29">
         <v>154</v>
       </c>
@@ -9600,7 +9475,7 @@
       <c r="M157" s="15"/>
       <c r="N157" s="20"/>
     </row>
-    <row r="158" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A158" s="29">
         <v>155</v>
       </c>
@@ -9642,7 +9517,7 @@
       </c>
       <c r="N158" s="20"/>
     </row>
-    <row r="159" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A159" s="29">
         <v>156</v>
       </c>
@@ -9684,7 +9559,7 @@
       </c>
       <c r="N159" s="20"/>
     </row>
-    <row r="160" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A160" s="29">
         <v>157</v>
       </c>
@@ -9745,162 +9620,99 @@
       <c r="N161" s="53"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G158:G160 G1:G5 G112:G128 G151:G156 G133:G149 G12:G26 G31:G33 G36:G68">
-    <cfRule type="expression" dxfId="70" priority="107">
+  <conditionalFormatting sqref="G1:G11">
+    <cfRule type="expression" dxfId="22" priority="26">
+      <formula>AND(ISNUMBER(SEARCH("Vacant", G1)),NOT(ISNUMBER(SEARCH("-&gt;",G1))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="25">
       <formula>AND(ISNUMBER(SEARCH("Vacant", G1)),(ISNUMBER(SEARCH("-&gt;",G1))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="108">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G1)),NOT(ISNUMBER(SEARCH("-&gt;",G1))))</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G35">
+    <cfRule type="endsWith" dxfId="20" priority="2" operator="endsWith" text="vacant}">
+      <formula>RIGHT(G1,LEN("vacant}"))="vacant}"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G27 G10 G7:G8 G29">
-    <cfRule type="expression" dxfId="68" priority="57">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G7)),(ISNUMBER(SEARCH("-&gt;",G7))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="58">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G7)),NOT(ISNUMBER(SEARCH("-&gt;",G7))))</formula>
+  <conditionalFormatting sqref="G2:G160">
+    <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="vacant} -&gt;">
+      <formula>NOT(ISERROR(SEARCH("vacant} -&gt;",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G157">
-    <cfRule type="expression" dxfId="66" priority="53">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G157)),(ISNUMBER(SEARCH("-&gt;",G157))))</formula>
+  <conditionalFormatting sqref="G12:G27">
+    <cfRule type="expression" dxfId="18" priority="58">
+      <formula>AND(ISNUMBER(SEARCH("Vacant", G12)),NOT(ISNUMBER(SEARCH("-&gt;",G12))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="54">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G157)),NOT(ISNUMBER(SEARCH("-&gt;",G157))))</formula>
+    <cfRule type="expression" dxfId="17" priority="57">
+      <formula>AND(ISNUMBER(SEARCH("Vacant", G12)),(ISNUMBER(SEARCH("-&gt;",G12))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25">
-    <cfRule type="expression" dxfId="64" priority="51">
+    <cfRule type="expression" dxfId="16" priority="52">
+      <formula>AND(ISNUMBER(SEARCH("Vacant", G25)),NOT(ISNUMBER(SEARCH("-&gt;",G25))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="51">
       <formula>AND(ISNUMBER(SEARCH("Vacant", G25)),(ISNUMBER(SEARCH("-&gt;",G25))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="52">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G25)),NOT(ISNUMBER(SEARCH("-&gt;",G25))))</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G28">
-    <cfRule type="expression" dxfId="62" priority="49">
+  <conditionalFormatting sqref="G28:G35">
+    <cfRule type="expression" dxfId="14" priority="3">
       <formula>AND(ISNUMBER(SEARCH("Vacant", G28)),(ISNUMBER(SEARCH("-&gt;",G28))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="50">
+    <cfRule type="expression" dxfId="13" priority="4">
       <formula>AND(ISNUMBER(SEARCH("Vacant", G28)),NOT(ISNUMBER(SEARCH("-&gt;",G28))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G150">
-    <cfRule type="expression" dxfId="60" priority="41">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G150)),(ISNUMBER(SEARCH("-&gt;",G150))))</formula>
+  <conditionalFormatting sqref="G36:G41">
+    <cfRule type="expression" dxfId="12" priority="20">
+      <formula>AND(ISNUMBER(SEARCH("Vacant", G36)),NOT(ISNUMBER(SEARCH("-&gt;",G36))))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="42">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G150)),NOT(ISNUMBER(SEARCH("-&gt;",G150))))</formula>
+    <cfRule type="expression" dxfId="11" priority="19">
+      <formula>AND(ISNUMBER(SEARCH("Vacant", G36)),(ISNUMBER(SEARCH("-&gt;",G36))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G36:G68 G112:G128">
+    <cfRule type="expression" dxfId="10" priority="108">
+      <formula>AND(ISNUMBER(SEARCH("Vacant", G36)),NOT(ISNUMBER(SEARCH("-&gt;",G36))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="107">
+      <formula>AND(ISNUMBER(SEARCH("Vacant", G36)),(ISNUMBER(SEARCH("-&gt;",G36))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G36:G1048576">
+    <cfRule type="endsWith" dxfId="8" priority="14" operator="endsWith" text="vacant}">
+      <formula>RIGHT(G36,LEN("vacant}"))="vacant}"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G62">
+    <cfRule type="expression" dxfId="7" priority="18">
+      <formula>AND(ISNUMBER(SEARCH("Vacant", G62)),NOT(ISNUMBER(SEARCH("-&gt;",G62))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="17">
+      <formula>AND(ISNUMBER(SEARCH("Vacant", G62)),(ISNUMBER(SEARCH("-&gt;",G62))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G65">
+    <cfRule type="expression" dxfId="5" priority="15">
+      <formula>AND(ISNUMBER(SEARCH("Vacant", G65)),(ISNUMBER(SEARCH("-&gt;",G65))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="16">
+      <formula>AND(ISNUMBER(SEARCH("Vacant", G65)),NOT(ISNUMBER(SEARCH("-&gt;",G65))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G133:G160">
+    <cfRule type="expression" dxfId="3" priority="42">
+      <formula>AND(ISNUMBER(SEARCH("Vacant", G133)),NOT(ISNUMBER(SEARCH("-&gt;",G133))))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="41">
+      <formula>AND(ISNUMBER(SEARCH("Vacant", G133)),(ISNUMBER(SEARCH("-&gt;",G133))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G137:G140">
-    <cfRule type="expression" dxfId="58" priority="37">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G137)),(ISNUMBER(SEARCH("-&gt;",G137))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="57" priority="38">
+    <cfRule type="expression" dxfId="1" priority="38">
       <formula>AND(ISNUMBER(SEARCH("Vacant", G137)),NOT(ISNUMBER(SEARCH("-&gt;",G137))))</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G9">
-    <cfRule type="expression" dxfId="56" priority="33">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G9)),(ISNUMBER(SEARCH("-&gt;",G9))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="55" priority="34">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G9)),NOT(ISNUMBER(SEARCH("-&gt;",G9))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G11">
-    <cfRule type="expression" dxfId="54" priority="31">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G11)),(ISNUMBER(SEARCH("-&gt;",G11))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="53" priority="32">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G11)),NOT(ISNUMBER(SEARCH("-&gt;",G11))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
-    <cfRule type="expression" dxfId="52" priority="25">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G6)),(ISNUMBER(SEARCH("-&gt;",G6))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="51" priority="26">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G6)),NOT(ISNUMBER(SEARCH("-&gt;",G6))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G30">
-    <cfRule type="expression" dxfId="50" priority="21">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G30)),(ISNUMBER(SEARCH("-&gt;",G30))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="49" priority="22">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G30)),NOT(ISNUMBER(SEARCH("-&gt;",G30))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G36:G41">
-    <cfRule type="expression" dxfId="48" priority="19">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G36)),(ISNUMBER(SEARCH("-&gt;",G36))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="47" priority="20">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G36)),NOT(ISNUMBER(SEARCH("-&gt;",G36))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G62">
-    <cfRule type="expression" dxfId="46" priority="17">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G62)),(ISNUMBER(SEARCH("-&gt;",G62))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="45" priority="18">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G62)),NOT(ISNUMBER(SEARCH("-&gt;",G62))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G65">
-    <cfRule type="expression" dxfId="44" priority="15">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G65)),(ISNUMBER(SEARCH("-&gt;",G65))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="16">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G65)),NOT(ISNUMBER(SEARCH("-&gt;",G65))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G33 G36:G1048576">
-    <cfRule type="endsWith" dxfId="42" priority="14" operator="endsWith" text="vacant}">
-      <formula>RIGHT(G1,LEN("vacant}"))="vacant}"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G33 G36:G160">
-    <cfRule type="containsText" dxfId="41" priority="13" operator="containsText" text="vacant} -&gt;">
-      <formula>NOT(ISERROR(SEARCH("vacant} -&gt;",G2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="expression" dxfId="40" priority="7">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G34)),(ISNUMBER(SEARCH("-&gt;",G34))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="39" priority="8">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G34)),NOT(ISNUMBER(SEARCH("-&gt;",G34))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="endsWith" dxfId="38" priority="6" operator="endsWith" text="vacant}">
-      <formula>RIGHT(G34,LEN("vacant}"))="vacant}"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="containsText" dxfId="37" priority="5" operator="containsText" text="vacant} -&gt;">
-      <formula>NOT(ISERROR(SEARCH("vacant} -&gt;",G34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
-    <cfRule type="expression" dxfId="36" priority="3">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G35)),(ISNUMBER(SEARCH("-&gt;",G35))))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="35" priority="4">
-      <formula>AND(ISNUMBER(SEARCH("Vacant", G35)),NOT(ISNUMBER(SEARCH("-&gt;",G35))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
-    <cfRule type="endsWith" dxfId="34" priority="2" operator="endsWith" text="vacant}">
-      <formula>RIGHT(G35,LEN("vacant}"))="vacant}"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
-    <cfRule type="containsText" dxfId="33" priority="1" operator="containsText" text="vacant} -&gt;">
-      <formula>NOT(ISERROR(SEARCH("vacant} -&gt;",G35)))</formula>
+    <cfRule type="expression" dxfId="0" priority="37">
+      <formula>AND(ISNUMBER(SEARCH("Vacant", G137)),(ISNUMBER(SEARCH("-&gt;",G137))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>